<commit_message>
Updated test objects for new output options
</commit_message>
<xml_diff>
--- a/RPackageSource/inst/extdata/test_objects/testData.xlsx
+++ b/RPackageSource/inst/extdata/test_objects/testData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="metaBolites" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="subjectmetAbolites" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="sUbjectdata" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="varmaP" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="modeLs" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="modeloptioNs" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="mEtabolites" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="subjeCtmetabolites" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="subjEctdata" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="vaRmap" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="modEls" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="mOdeloptions" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t xml:space="preserve">metabid</t>
   </si>
@@ -382,16 +382,16 @@
     <t xml:space="preserve">categoricAl</t>
   </si>
   <si>
-    <t xml:space="preserve">mOdel</t>
+    <t xml:space="preserve">modEl</t>
   </si>
   <si>
-    <t xml:space="preserve">outcoMes</t>
+    <t xml:space="preserve">oUtcomes</t>
   </si>
   <si>
-    <t xml:space="preserve">exPosure</t>
+    <t xml:space="preserve">eXposure</t>
   </si>
   <si>
-    <t xml:space="preserve">adjustmenT</t>
+    <t xml:space="preserve">adjusTment</t>
   </si>
   <si>
     <t xml:space="preserve">stRatification</t>
@@ -400,7 +400,7 @@
     <t xml:space="preserve">wHere</t>
   </si>
   <si>
-    <t xml:space="preserve">modelSpec</t>
+    <t xml:space="preserve">moDelspec</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -409,7 +409,7 @@
     <t xml:space="preserve">alL metabolites</t>
   </si>
   <si>
-    <t xml:space="preserve">cat1 cOnt1</t>
+    <t xml:space="preserve">cat1 conT1</t>
   </si>
   <si>
     <t xml:space="preserve">new_corr</t>
@@ -424,7 +424,7 @@
     <t xml:space="preserve">cont1</t>
   </si>
   <si>
-    <t xml:space="preserve">cont2 Cont3_corr2</t>
+    <t xml:space="preserve">cont2 cont3_coRr2</t>
   </si>
   <si>
     <t xml:space="preserve">lm</t>
@@ -436,7 +436,7 @@
     <t xml:space="preserve">all metAbolites</t>
   </si>
   <si>
-    <t xml:space="preserve">cat1 cat1_dup</t>
+    <t xml:space="preserve">cat1 cAt1_dup</t>
   </si>
   <si>
     <t xml:space="preserve">glm_linear</t>
@@ -451,7 +451,7 @@
     <t xml:space="preserve">cont2</t>
   </si>
   <si>
-    <t xml:space="preserve">cat2 caT3_2</t>
+    <t xml:space="preserve">cat2 cat3_2</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">all metabOlites</t>
   </si>
   <si>
-    <t xml:space="preserve">cOnt4_miss &gt; 0</t>
+    <t xml:space="preserve">cont4_mIss &gt; 0</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
@@ -484,22 +484,10 @@
     <t xml:space="preserve">cOnt1</t>
   </si>
   <si>
-    <t xml:space="preserve">orig_corr</t>
+    <t xml:space="preserve">caT1</t>
   </si>
   <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alliin fUcose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydantoin_5_prOpionic_acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catAb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glm.log2</t>
+    <t xml:space="preserve">orig_corr</t>
   </si>
   <si>
     <t xml:space="preserve">MODELSPEC</t>
@@ -528,20 +516,11 @@
   <si>
     <t xml:space="preserve">runCorr</t>
   </si>
-  <si>
-    <t xml:space="preserve">weights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">offset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cont3_corr2</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -860,10 +839,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -1160,10 +1139,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -18477,10 +18456,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -34519,10 +34498,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -34701,10 +34680,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -34883,36 +34862,36 @@
         <v>154</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
       <c r="F8" t="s">
         <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
         <v>91</v>
       </c>
       <c r="G9" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -34922,25 +34901,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2">
@@ -34948,7 +34927,7 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>91</v>
@@ -34976,7 +34955,7 @@
         <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>91</v>
@@ -34990,21 +34969,21 @@
         <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
         <v>91</v>
@@ -35015,44 +34994,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D9" t="s">
-        <v>172</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>